<commit_message>
add histogram and feature selection method
</commit_message>
<xml_diff>
--- a/clustercenters.xlsx
+++ b/clustercenters.xlsx
@@ -470,22 +470,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.092182727240839</v>
+        <v>1.0158</v>
       </c>
       <c r="C2" t="n">
-        <v>2.07375111864537</v>
+        <v>2.1627</v>
       </c>
       <c r="D2" t="n">
-        <v>4.102469685736769</v>
+        <v>6.3036</v>
       </c>
       <c r="E2" t="n">
-        <v>17.45059884338514</v>
+        <v>26.248</v>
       </c>
       <c r="F2" t="n">
-        <v>6.481555960307865</v>
+        <v>11.0382</v>
       </c>
       <c r="G2" t="n">
-        <v>5.220418050833767</v>
+        <v>4.5989</v>
       </c>
     </row>
     <row r="3">
@@ -493,22 +493,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.122040415136985</v>
+        <v>1.1352</v>
       </c>
       <c r="C3" t="n">
-        <v>2.15801175071811</v>
+        <v>2.0394</v>
       </c>
       <c r="D3" t="n">
-        <v>5.165827347726465</v>
+        <v>5.464</v>
       </c>
       <c r="E3" t="n">
-        <v>21.79853130770023</v>
+        <v>21.9319</v>
       </c>
       <c r="F3" t="n">
-        <v>8.46846956693417</v>
+        <v>8.6128</v>
       </c>
       <c r="G3" t="n">
-        <v>6.01070216848805</v>
+        <v>5.7864</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.050121094324648</v>
+        <v>1.236</v>
       </c>
       <c r="C4" t="n">
-        <v>2.182203802658533</v>
+        <v>1.8717</v>
       </c>
       <c r="D4" t="n">
-        <v>6.311693334148417</v>
+        <v>4.508</v>
       </c>
       <c r="E4" t="n">
-        <v>26.11092111789246</v>
+        <v>17.6459</v>
       </c>
       <c r="F4" t="n">
-        <v>10.80509274902625</v>
+        <v>6.746</v>
       </c>
       <c r="G4" t="n">
-        <v>4.592266472065333</v>
+        <v>6.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update flow, method, and readme
</commit_message>
<xml_diff>
--- a/clustercenters.xlsx
+++ b/clustercenters.xlsx
@@ -472,71 +472,71 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7.8815</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>12.4855</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>10.6501</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3835</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>23.7964</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>20.9025</v>
+        <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>5.8103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13.6753</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>3.1785</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>6.9091</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>9.1191</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>19.3108</v>
+        <v>19</v>
       </c>
       <c r="F3" t="n">
-        <v>15.1198</v>
+        <v>7</v>
       </c>
       <c r="G3" t="n">
-        <v>8.093500000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15.0575</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>12.5237</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>16.1016</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>13.0077</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>18.6132</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
-        <v>24.2139</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>7.165</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>